<commit_message>
create updated version of mem_intf_model and invert colr_en signal
</commit_message>
<xml_diff>
--- a/docs/memory_calcs.xlsx
+++ b/docs/memory_calcs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t xml:space="preserve">RESOLUTION</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">ARTY-A7 BRAM</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTY-A7 DDR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Width:</t>
   </si>
   <si>
@@ -44,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Total pxls:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MB</t>
   </si>
   <si>
     <t xml:space="preserve">Bitmaps</t>
@@ -101,15 +107,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -135,6 +147,20 @@
       <left/>
       <right style="hair"/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -199,12 +225,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -216,15 +242,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -232,7 +266,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -240,11 +274,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -257,6 +291,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB4C7DC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -265,10 +359,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:I13"/>
+  <dimension ref="B2:K13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
+      <selection pane="topLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -285,59 +379,90 @@
         <v>1</v>
       </c>
       <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>640</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I3" s="3" t="n">
         <v>4860000</v>
       </c>
+      <c r="J3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <f aca="false">K4*8</f>
+        <v>2048000000</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>480</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" s="3" t="n">
         <f aca="false">I3/8</f>
         <v>607500</v>
       </c>
+      <c r="J4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <f aca="false">K5*1000</f>
+        <v>256000000</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="H5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="6" t="n">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="H5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="8" t="n">
         <f aca="false">I4/1000</f>
         <v>607.5</v>
       </c>
+      <c r="J5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <f aca="false">K6*1000</f>
+        <v>256000</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="6" t="n">
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8" t="n">
         <f aca="false">C3*C4</f>
         <v>307200</v>
       </c>
+      <c r="J6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="8" t="n">
+        <v>256</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -349,12 +474,12 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="7"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -362,23 +487,23 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8" t="s">
-        <v>11</v>
+      <c r="B10" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="9" t="n">
+      <c r="D10" s="9"/>
+      <c r="E10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="G10" s="9" t="n">
+      <c r="G10" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="H10" s="9" t="n">
+      <c r="H10" s="11" t="n">
         <v>3</v>
       </c>
       <c r="I10" s="3" t="n">
@@ -386,26 +511,26 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="8" t="s">
-        <v>3</v>
+      <c r="B11" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="C11" s="3" t="n">
         <f aca="false">C6</f>
         <v>307200</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="9" t="n">
+      <c r="D11" s="9"/>
+      <c r="E11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="11" t="n">
         <f aca="false">F10*3*$C$6</f>
         <v>921600</v>
       </c>
-      <c r="G11" s="9" t="n">
+      <c r="G11" s="11" t="n">
         <f aca="false">G10*3*$C$6</f>
         <v>1843200</v>
       </c>
-      <c r="H11" s="9" t="n">
+      <c r="H11" s="11" t="n">
         <f aca="false">H10*3*$C$6</f>
         <v>2764800</v>
       </c>
@@ -415,26 +540,26 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="8" t="s">
-        <v>5</v>
+      <c r="B12" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="C12" s="3" t="n">
         <f aca="false">C11/8</f>
         <v>38400</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="9" t="n">
+      <c r="D12" s="9"/>
+      <c r="E12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="11" t="n">
         <f aca="false">F11/8</f>
         <v>115200</v>
       </c>
-      <c r="G12" s="9" t="n">
+      <c r="G12" s="11" t="n">
         <f aca="false">G11/8</f>
         <v>230400</v>
       </c>
-      <c r="H12" s="9" t="n">
+      <c r="H12" s="11" t="n">
         <f aca="false">H11/8</f>
         <v>345600</v>
       </c>
@@ -444,38 +569,39 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="6" t="n">
+      <c r="B13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="8" t="n">
         <f aca="false">C12/1000</f>
         <v>38.4</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="11" t="n">
+      <c r="D13" s="9"/>
+      <c r="E13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="13" t="n">
         <f aca="false">F12/1000</f>
         <v>115.2</v>
       </c>
-      <c r="G13" s="11" t="n">
+      <c r="G13" s="13" t="n">
         <f aca="false">G12/1000</f>
         <v>230.4</v>
       </c>
-      <c r="H13" s="11" t="n">
+      <c r="H13" s="13" t="n">
         <f aca="false">H12/1000</f>
         <v>345.6</v>
       </c>
-      <c r="I13" s="6" t="n">
+      <c r="I13" s="8" t="n">
         <f aca="false">I12/1000</f>
         <v>460.8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B8:I8"/>
     <mergeCell ref="B9:C9"/>

</xml_diff>

<commit_message>
add memory initialisation files and add code to initialise ram
</commit_message>
<xml_diff>
--- a/docs/memory_calcs.xlsx
+++ b/docs/memory_calcs.xlsx
@@ -77,6 +77,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -99,12 +100,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -362,12 +365,12 @@
   <dimension ref="B2:K13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
+      <selection pane="topLeft" activeCell="O19" activeCellId="0" sqref="O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="1.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="1.93"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update memory intf model to use corrected bufferring scheme
</commit_message>
<xml_diff>
--- a/docs/memory_calcs.xlsx
+++ b/docs/memory_calcs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t xml:space="preserve">RESOLUTION</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">ARTY-A7 DDR</t>
   </si>
   <si>
+    <t xml:space="preserve">ZYBO Z7010 BRAM</t>
+  </si>
+  <si>
     <t xml:space="preserve">Width:</t>
   </si>
   <si>
@@ -62,6 +65,57 @@
   </si>
   <si>
     <t xml:space="preserve">Bit-Depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tile Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBuff (1) b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBuff (1) B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBuff (1) kB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBuff Tot. b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBuff Tot. B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBuff Tot. kB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiles p Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt; needs to be a power of 2 for easy AXI address translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fbuff b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fbuff B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fbuff kB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fbuff Wdth b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fbuff Dpth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addr Wdth b</t>
   </si>
 </sst>
 </file>
@@ -110,7 +164,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,8 +177,14 @@
         <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FFB4C7DC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="24">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -200,6 +260,97 @@
       <right/>
       <top/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -228,7 +379,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -265,6 +416,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -273,16 +428,120 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -332,7 +591,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -362,15 +621,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:K13"/>
+  <dimension ref="B2:M36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O19" activeCellId="0" sqref="O19"/>
+      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="1.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="1.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.49"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,78 +646,101 @@
         <v>2</v>
       </c>
       <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>640</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I3" s="3" t="n">
         <v>4860000</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K3" s="5" t="n">
         <f aca="false">K4*8</f>
         <v>2048000000</v>
       </c>
+      <c r="L3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>4860000</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>480</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I4" s="3" t="n">
         <f aca="false">I3/8</f>
         <v>607500</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K4" s="3" t="n">
         <f aca="false">K5*1000</f>
         <v>256000000</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <f aca="false">M3/8</f>
+        <v>607500</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="H5" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I5" s="8" t="n">
         <f aca="false">I4/1000</f>
         <v>607.5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K5" s="3" t="n">
         <f aca="false">K6*1000</f>
         <v>256000</v>
       </c>
+      <c r="L5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="8" t="n">
+        <v>270</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="8" t="n">
         <f aca="false">C3*C4</f>
         <v>307200</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K6" s="8" t="n">
         <v>256</v>
@@ -465,7 +748,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -474,39 +757,43 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="9"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="10" t="s">
-        <v>13</v>
+      <c r="B10" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="11" t="n">
+      <c r="D10" s="10"/>
+      <c r="E10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="G10" s="11" t="n">
+      <c r="G10" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="H10" s="11" t="n">
+      <c r="H10" s="9" t="n">
         <v>3</v>
       </c>
       <c r="I10" s="3" t="n">
@@ -514,26 +801,26 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="10" t="s">
-        <v>4</v>
+      <c r="B11" s="11" t="s">
+        <v>5</v>
       </c>
       <c r="C11" s="3" t="n">
         <f aca="false">C6</f>
         <v>307200</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="11" t="n">
+      <c r="D11" s="10"/>
+      <c r="E11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="9" t="n">
         <f aca="false">F10*3*$C$6</f>
         <v>921600</v>
       </c>
-      <c r="G11" s="11" t="n">
+      <c r="G11" s="9" t="n">
         <f aca="false">G10*3*$C$6</f>
         <v>1843200</v>
       </c>
-      <c r="H11" s="11" t="n">
+      <c r="H11" s="9" t="n">
         <f aca="false">H10*3*$C$6</f>
         <v>2764800</v>
       </c>
@@ -543,26 +830,26 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="10" t="s">
-        <v>6</v>
+      <c r="B12" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="C12" s="3" t="n">
         <f aca="false">C11/8</f>
         <v>38400</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="11" t="n">
+      <c r="D12" s="10"/>
+      <c r="E12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="9" t="n">
         <f aca="false">F11/8</f>
         <v>115200</v>
       </c>
-      <c r="G12" s="11" t="n">
+      <c r="G12" s="9" t="n">
         <f aca="false">G11/8</f>
         <v>230400</v>
       </c>
-      <c r="H12" s="11" t="n">
+      <c r="H12" s="9" t="n">
         <f aca="false">H11/8</f>
         <v>345600</v>
       </c>
@@ -573,15 +860,15 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="8" t="n">
         <f aca="false">C12/1000</f>
         <v>38.4</v>
       </c>
-      <c r="D13" s="9"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F13" s="13" t="n">
         <f aca="false">F12/1000</f>
@@ -600,16 +887,431 @@
         <v>460.8</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="G18" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" s="21" t="n">
+        <v>12</v>
+      </c>
+      <c r="F19" s="22" t="n">
+        <v>12</v>
+      </c>
+      <c r="G19" s="21" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="20" t="n">
+        <f aca="false">(C6*C19) / (C18^2)</f>
+        <v>76800</v>
+      </c>
+      <c r="E20" s="21" t="n">
+        <f aca="false">($C$6 * E19) / (E18^2)</f>
+        <v>921600</v>
+      </c>
+      <c r="F20" s="22" t="n">
+        <f aca="false">($C$6 * F19) / (F18^2)</f>
+        <v>230400</v>
+      </c>
+      <c r="G20" s="21" t="n">
+        <f aca="false">($C$6 * G19) / (G18^2)</f>
+        <v>147456</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="20" t="n">
+        <f aca="false">C20/8</f>
+        <v>9600</v>
+      </c>
+      <c r="E21" s="21" t="n">
+        <f aca="false">E20/8</f>
+        <v>115200</v>
+      </c>
+      <c r="F21" s="22" t="n">
+        <f aca="false">F20/8</f>
+        <v>28800</v>
+      </c>
+      <c r="G21" s="21" t="n">
+        <f aca="false">G20/8</f>
+        <v>18432</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="24" t="n">
+        <f aca="false">C21/1000</f>
+        <v>9.6</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26" t="n">
+        <f aca="false">E21/1000</f>
+        <v>115.2</v>
+      </c>
+      <c r="F22" s="27" t="n">
+        <f aca="false">F21/1000</f>
+        <v>28.8</v>
+      </c>
+      <c r="G22" s="26" t="n">
+        <f aca="false">G21/1000</f>
+        <v>18.432</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="28" t="n">
+        <f aca="false">C19*($C$3/C18)</f>
+        <v>640</v>
+      </c>
+      <c r="E24" s="29" t="n">
+        <f aca="false">E19*($C$3/E18)</f>
+        <v>3840</v>
+      </c>
+      <c r="F24" s="30" t="n">
+        <f aca="false">F19*($C$3/F18)</f>
+        <v>1920</v>
+      </c>
+      <c r="G24" s="29" t="n">
+        <f aca="false">G19*($C$3/G18)</f>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="28" t="n">
+        <f aca="false">C24/8</f>
+        <v>80</v>
+      </c>
+      <c r="E25" s="32" t="n">
+        <f aca="false">E24/8</f>
+        <v>480</v>
+      </c>
+      <c r="F25" s="30" t="n">
+        <f aca="false">F24/8</f>
+        <v>240</v>
+      </c>
+      <c r="G25" s="32" t="n">
+        <f aca="false">G24/8</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="28" t="n">
+        <f aca="false">C25/1000</f>
+        <v>0.08</v>
+      </c>
+      <c r="E26" s="32" t="n">
+        <f aca="false">E25/1000</f>
+        <v>0.48</v>
+      </c>
+      <c r="F26" s="30" t="n">
+        <f aca="false">F25/1000</f>
+        <v>0.24</v>
+      </c>
+      <c r="G26" s="32" t="n">
+        <f aca="false">G25/1000</f>
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="33" t="n">
+        <f aca="false">C24*2</f>
+        <v>1280</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="E27" s="29" t="n">
+        <f aca="false">E24*2</f>
+        <v>7680</v>
+      </c>
+      <c r="F27" s="34" t="n">
+        <f aca="false">F24*2</f>
+        <v>3840</v>
+      </c>
+      <c r="G27" s="29" t="n">
+        <f aca="false">G24*2</f>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="28" t="n">
+        <f aca="false">C27/8</f>
+        <v>160</v>
+      </c>
+      <c r="E28" s="32" t="n">
+        <f aca="false">E27/8</f>
+        <v>960</v>
+      </c>
+      <c r="F28" s="30" t="n">
+        <f aca="false">F27/8</f>
+        <v>480</v>
+      </c>
+      <c r="G28" s="32" t="n">
+        <f aca="false">G27/8</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="24" t="n">
+        <f aca="false">C28/1000</f>
+        <v>0.16</v>
+      </c>
+      <c r="D29" s="25"/>
+      <c r="E29" s="26" t="n">
+        <f aca="false">E28/1000</f>
+        <v>0.96</v>
+      </c>
+      <c r="F29" s="36" t="n">
+        <f aca="false">F28/1000</f>
+        <v>0.48</v>
+      </c>
+      <c r="G29" s="26" t="n">
+        <f aca="false">G28/1000</f>
+        <v>0.384</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="D30" s="25"/>
+      <c r="E30" s="26" t="n">
+        <v>4</v>
+      </c>
+      <c r="F30" s="36" t="n">
+        <v>4</v>
+      </c>
+      <c r="G30" s="26" t="n">
+        <v>4</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="33" t="n">
+        <f aca="false">($C$3*$C$4*C19)/(C18*C18)</f>
+        <v>76800</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="29" t="n">
+        <f aca="false">($C$3*$C$4*E19)/(E18*E18)</f>
+        <v>921600</v>
+      </c>
+      <c r="F31" s="34" t="n">
+        <f aca="false">($C$3*$C$4*F19)/(F18*F18)</f>
+        <v>230400</v>
+      </c>
+      <c r="G31" s="29" t="n">
+        <f aca="false">($C$3*$C$4*G19)/(G18*G18)</f>
+        <v>147456</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="28" t="n">
+        <f aca="false">C31/8</f>
+        <v>9600</v>
+      </c>
+      <c r="E32" s="32" t="n">
+        <f aca="false">E31/8</f>
+        <v>115200</v>
+      </c>
+      <c r="F32" s="30" t="n">
+        <f aca="false">F31/8</f>
+        <v>28800</v>
+      </c>
+      <c r="G32" s="32" t="n">
+        <f aca="false">G31/8</f>
+        <v>18432</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="24" t="n">
+        <f aca="false">C32/1000</f>
+        <v>9.6</v>
+      </c>
+      <c r="D33" s="25"/>
+      <c r="E33" s="26" t="n">
+        <f aca="false">E32/1000</f>
+        <v>115.2</v>
+      </c>
+      <c r="F33" s="36" t="n">
+        <f aca="false">F32/1000</f>
+        <v>28.8</v>
+      </c>
+      <c r="G33" s="26" t="n">
+        <f aca="false">G32/1000</f>
+        <v>18.432</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="29" t="n">
+        <f aca="false">C30*C19</f>
+        <v>16</v>
+      </c>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29" t="n">
+        <f aca="false">E30*E19</f>
+        <v>48</v>
+      </c>
+      <c r="F34" s="29" t="n">
+        <f aca="false">F30*F19</f>
+        <v>48</v>
+      </c>
+      <c r="G34" s="29" t="n">
+        <f aca="false">G30*G19</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="32" t="n">
+        <f aca="false">($C$3 * $C$4 * C19)/((C18*C18)*C34)</f>
+        <v>4800</v>
+      </c>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32" t="n">
+        <f aca="false">($C$3 * $C$4 * E19)/((E18*E18)*E34)</f>
+        <v>19200</v>
+      </c>
+      <c r="F35" s="32" t="n">
+        <f aca="false">($C$3 * $C$4 * F19)/((F18*F18)*F34)</f>
+        <v>4800</v>
+      </c>
+      <c r="G35" s="32" t="n">
+        <f aca="false">($C$3 * $C$4 * G19)/((G18*G18)*G34)</f>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="26" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(LOG(C35,2))</f>
+        <v>13</v>
+      </c>
+      <c r="D36" s="25"/>
+      <c r="E36" s="40" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(LOG(E35,2))</f>
+        <v>15</v>
+      </c>
+      <c r="F36" s="26" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(LOG(F35,2))</f>
+        <v>13</v>
+      </c>
+      <c r="G36" s="24" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(LOG(G35,2))</f>
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="13">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B8:I8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:D13"/>
     <mergeCell ref="E9:I9"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B23:G23"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
move reset sync to simulation only, update diagram and add calcs for AXI addressing
</commit_message>
<xml_diff>
--- a/docs/memory_calcs.xlsx
+++ b/docs/memory_calcs.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="AXI2MEM_analysis" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t xml:space="preserve">RESOLUTION</t>
   </si>
@@ -116,6 +117,48 @@
   </si>
   <si>
     <t xml:space="preserve">Addr Wdth b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tile size:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pxl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each AXI address is ½ of a frame buffer line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To convert address, divide it by 4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If address is odd, it is upper half (bit 0 -&gt; 23 of AXI map to bit 24 → 47 of frame buff)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If address is even, it is lower half (bit 0 -&gt; 23 of AXI map to bit 0 → 23 of frame buff)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AXI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intermediate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…</t>
   </si>
 </sst>
 </file>
@@ -184,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -350,6 +393,13 @@
       <left style="thin"/>
       <right/>
       <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -379,7 +429,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -542,6 +592,34 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -623,11 +701,11 @@
   </sheetPr>
   <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M29" activeCellId="0" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="1.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.49"/>
@@ -1321,4 +1399,317 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:E32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="42" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="43"/>
+      <c r="D5" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="45" t="n">
+        <v>480</v>
+      </c>
+      <c r="E6" s="45" t="n">
+        <f aca="false">D6/C2</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="45" t="n">
+        <v>640</v>
+      </c>
+      <c r="E7" s="45" t="n">
+        <f aca="false">D7/C2</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="45" t="n">
+        <f aca="false">D7*D6</f>
+        <v>307200</v>
+      </c>
+      <c r="E8" s="45" t="n">
+        <f aca="false">E7*E6</f>
+        <v>19200</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="45" t="n">
+        <f aca="false">C18/4</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="47" t="n">
+        <f aca="false">IF((ISODD(D18)), (D18-1)/2, D18/2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="45" t="n">
+        <v>4</v>
+      </c>
+      <c r="D19" s="45" t="n">
+        <f aca="false">C19/4</f>
+        <v>1</v>
+      </c>
+      <c r="E19" s="47" t="n">
+        <f aca="false">IF((ISODD(D19)), (D19-1)/2, D19/2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="45" t="n">
+        <v>8</v>
+      </c>
+      <c r="D20" s="45" t="n">
+        <f aca="false">C20/4</f>
+        <v>2</v>
+      </c>
+      <c r="E20" s="47" t="n">
+        <f aca="false">IF((ISODD(D20)), (D20-1)/2, D20/2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="45" t="n">
+        <f aca="false">C20+4</f>
+        <v>12</v>
+      </c>
+      <c r="D21" s="45" t="n">
+        <f aca="false">C21/4</f>
+        <v>3</v>
+      </c>
+      <c r="E21" s="47" t="n">
+        <f aca="false">IF((ISODD(D21)), (D21-1)/2, D21/2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="45" t="n">
+        <f aca="false">C21+4</f>
+        <v>16</v>
+      </c>
+      <c r="D22" s="45" t="n">
+        <f aca="false">C22/4</f>
+        <v>4</v>
+      </c>
+      <c r="E22" s="47" t="n">
+        <f aca="false">IF((ISODD(D22)), (D22-1)/2, D22/2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="45" t="n">
+        <f aca="false">C22+4</f>
+        <v>20</v>
+      </c>
+      <c r="D23" s="45" t="n">
+        <f aca="false">C23/4</f>
+        <v>5</v>
+      </c>
+      <c r="E23" s="47" t="n">
+        <f aca="false">IF((ISODD(D23)), (D23-1)/2, D23/2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="45" t="n">
+        <f aca="false">C23+4</f>
+        <v>24</v>
+      </c>
+      <c r="D24" s="45" t="n">
+        <f aca="false">C24/4</f>
+        <v>6</v>
+      </c>
+      <c r="E24" s="47" t="n">
+        <f aca="false">IF((ISODD(D24)), (D24-1)/2, D24/2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="45" t="n">
+        <f aca="false">C24+4</f>
+        <v>28</v>
+      </c>
+      <c r="D25" s="45" t="n">
+        <f aca="false">C25/4</f>
+        <v>7</v>
+      </c>
+      <c r="E25" s="47" t="n">
+        <f aca="false">IF((ISODD(D25)), (D25-1)/2, D25/2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="45" t="n">
+        <f aca="false">C25+4</f>
+        <v>32</v>
+      </c>
+      <c r="D26" s="45" t="n">
+        <f aca="false">C26/4</f>
+        <v>8</v>
+      </c>
+      <c r="E26" s="47" t="n">
+        <f aca="false">IF((ISODD(D26)), (D26-1)/2, D26/2)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="45" t="n">
+        <f aca="false">C26+4</f>
+        <v>36</v>
+      </c>
+      <c r="D27" s="45" t="n">
+        <f aca="false">C27/4</f>
+        <v>9</v>
+      </c>
+      <c r="E27" s="47" t="n">
+        <f aca="false">IF((ISODD(D27)), (D27-1)/2, D27/2)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="45" t="n">
+        <f aca="false">C27+4</f>
+        <v>40</v>
+      </c>
+      <c r="D28" s="45" t="n">
+        <f aca="false">C28/4</f>
+        <v>10</v>
+      </c>
+      <c r="E28" s="47" t="n">
+        <f aca="false">IF((ISODD(D28)), (D28-1)/2, D28/2)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="45" t="n">
+        <f aca="false">C28+4</f>
+        <v>44</v>
+      </c>
+      <c r="D29" s="45" t="n">
+        <f aca="false">C29/4</f>
+        <v>11</v>
+      </c>
+      <c r="E29" s="47" t="n">
+        <f aca="false">IF((ISODD(D29)), (D29-1)/2, D29/2)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="45" t="n">
+        <f aca="false">C29+4</f>
+        <v>48</v>
+      </c>
+      <c r="D30" s="45" t="n">
+        <f aca="false">C30/4</f>
+        <v>12</v>
+      </c>
+      <c r="E30" s="47" t="n">
+        <f aca="false">IF((ISODD(D30)), (D30-1)/2, D30/2)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="45" t="n">
+        <f aca="false">(E8-1)*2*4</f>
+        <v>153592</v>
+      </c>
+      <c r="D32" s="45" t="n">
+        <f aca="false">C32/4</f>
+        <v>38398</v>
+      </c>
+      <c r="E32" s="47" t="n">
+        <f aca="false">IF((ISODD(D32)), (D32-1)/2, D32/2)</f>
+        <v>19199</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>